<commit_message>
updated function points with new uc change password
</commit_message>
<xml_diff>
--- a/documentation/FunctionPoints.xlsx
+++ b/documentation/FunctionPoints.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Documents\guesswhere\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Documents\guesswhere_doc\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF21333D-DD7D-4361-932D-09CD672D4E34}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C996B3E0-2D5E-4153-9CF3-16C64302172B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="26">
   <si>
     <t>Finished UC</t>
   </si>
@@ -92,6 +92,18 @@
   </si>
   <si>
     <t>Average</t>
+  </si>
+  <si>
+    <t>Change Password</t>
+  </si>
+  <si>
+    <t>21.75</t>
+  </si>
+  <si>
+    <t>Challenge User (actually)</t>
+  </si>
+  <si>
+    <t>Change Password (actually)</t>
   </si>
 </sst>
 </file>
@@ -927,6 +939,474 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Change Password</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>Change Password</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-A7A2-40BD-AB33-02AD58A60241}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>21.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-A7A2-40BD-AB33-02AD58A60241}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Challenge User (actually)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>Challenge User (actually)</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-A7A2-40BD-AB33-02AD58A60241}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$C$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>27.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-A7A2-40BD-AB33-02AD58A60241}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Change Password (actually)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{E5ABC988-640B-441D-B9A5-004B6238C12A}" type="SERIESNAME">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[DATENREIHENNAME]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="de-DE"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-A7A2-40BD-AB33-02AD58A60241}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>21.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-A7A2-40BD-AB33-02AD58A60241}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
@@ -943,6 +1423,7 @@
         <c:axId val="1611159823"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="12"/>
           <c:min val="3"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1899,6 +2380,21 @@
 </table>
 </file>
 
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{769B1146-3FF4-4062-A6AA-860ED78010A2}" name="Tabelle57" displayName="Tabelle57" ref="A42:F48" totalsRowShown="0">
+  <autoFilter ref="A42:F48" xr:uid="{769B1146-3FF4-4062-A6AA-860ED78010A2}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{63B073E2-88D3-4D3D-B651-46CE3B44C360}" name="Change Password"/>
+    <tableColumn id="2" xr3:uid="{66BA18B1-9D47-4990-B840-2ACCDEA59FDB}" name="DET"/>
+    <tableColumn id="3" xr3:uid="{4CFC7EA9-4382-4877-8105-B73FCECB7011}" name="RET"/>
+    <tableColumn id="4" xr3:uid="{FA136121-FA2B-4DAC-8C6D-1E9AF82BCB3A}" name="FTR"/>
+    <tableColumn id="5" xr3:uid="{EE97313F-2B4C-4CFD-AD79-E96DE70B3B79}" name="Resulting Complexity"/>
+    <tableColumn id="6" xr3:uid="{62698E58-AC44-42BD-8812-4B7D131604DF}" name="Count"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2162,15 +2658,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A4:C15"/>
+  <dimension ref="A4:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2243,6 +2739,39 @@
       </c>
       <c r="C15">
         <v>27.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16">
+        <v>7.3</v>
+      </c>
+      <c r="C16">
+        <v>21.75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18">
+        <v>11</v>
+      </c>
+      <c r="C18">
+        <v>27.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>21.75</v>
       </c>
     </row>
   </sheetData>
@@ -2253,10 +2782,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{323D2A8B-E2C6-481A-BAE0-A11C1B1169CA}">
-  <dimension ref="A2:F40"/>
+  <dimension ref="A2:F48"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView topLeftCell="A23" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2925,15 +3454,148 @@
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
     </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" t="s">
+        <v>16</v>
+      </c>
+      <c r="E42" t="s">
+        <v>17</v>
+      </c>
+      <c r="F42" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>11</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>20</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47" t="s">
+        <v>19</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>13</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="5">
+  <tableParts count="6">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>